<commit_message>
Partial version of guidebook now available
Write the initial version of the guide book. It's about half finished
but gets the user started with creating their dataless SEED files.
</commit_message>
<xml_diff>
--- a/Station_configuration_worksheet.xlsx
+++ b/Station_configuration_worksheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="66">
   <si>
     <t>Sensitivity/gain</t>
   </si>
@@ -211,6 +211,12 @@
   </si>
   <si>
     <t>Default value</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>2015,328,18:00:00.000</t>
   </si>
 </sst>
 </file>
@@ -248,7 +254,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +264,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,29 +292,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -594,14 +618,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="5" width="21.42578125" customWidth="1"/>
   </cols>
@@ -620,40 +644,40 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="8">
         <f>0.954</f>
         <v>0.95399999999999996</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="14"/>
-    </row>
-    <row r="8" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
         <v>20</v>
       </c>
@@ -662,7 +686,7 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -670,7 +694,7 @@
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>53</v>
       </c>
     </row>
@@ -678,7 +702,7 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="8">
         <v>42.716700000000003</v>
       </c>
     </row>
@@ -686,7 +710,7 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="8">
         <v>-84.231099999999998</v>
       </c>
     </row>
@@ -694,7 +718,7 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="8">
         <v>282</v>
       </c>
     </row>
@@ -702,7 +726,7 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -710,15 +734,15 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="4" t="s">
         <v>31</v>
       </c>
@@ -727,7 +751,7 @@
       <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -735,10 +759,10 @@
       <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="10">
         <v>0</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -746,10 +770,10 @@
       <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="10">
         <v>-90</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -757,15 +781,20 @@
       <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="8">
         <v>130.19999999999999</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="C23" s="1"/>
       <c r="D23" s="4" t="s">
         <v>19</v>
@@ -775,7 +804,7 @@
       <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="11">
         <v>2</v>
       </c>
       <c r="C24" s="1"/>
@@ -784,11 +813,11 @@
       <c r="A25" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="11">
         <v>1</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="6" t="s">
         <v>51</v>
       </c>
     </row>
@@ -796,13 +825,13 @@
       <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="8">
         <v>-4.9842000000000004</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -810,10 +839,10 @@
       <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="8">
         <v>-4.9842000000000004</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -823,7 +852,7 @@
       <c r="D28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -831,25 +860,25 @@
       <c r="A29" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="13">
         <v>386.4</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="14"/>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30" s="14">
         <v>5</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -862,26 +891,26 @@
       <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="13">
         <f>1/(digigain)*1000000</f>
         <v>1048218.0293501049</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="14"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33" s="14">
         <v>1</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -894,13 +923,13 @@
       <c r="A35" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="13">
         <v>1</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -908,13 +937,13 @@
       <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="11">
+      <c r="B36" s="14">
         <v>1</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -928,19 +957,19 @@
       <c r="A38" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="16">
         <f>B32*B29*B35</f>
         <v>405031446.5408805</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
       <c r="E40" s="4" t="s">
         <v>43</v>
       </c>
@@ -949,7 +978,7 @@
       <c r="A41" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -957,10 +986,10 @@
       <c r="A42" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="15">
         <v>0</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -968,10 +997,10 @@
       <c r="A43" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="15">
         <v>0</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -979,15 +1008,20 @@
       <c r="A44" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="8">
         <v>130.19999999999999</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
+      <c r="A45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="C45" s="1"/>
       <c r="D45" s="4" t="s">
         <v>19</v>
@@ -997,7 +1031,7 @@
       <c r="A46" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="7">
+      <c r="B46" s="11">
         <v>2</v>
       </c>
       <c r="C46" s="1"/>
@@ -1006,11 +1040,11 @@
       <c r="A47" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="11">
         <v>1</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="14" t="s">
+      <c r="D47" s="6" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1018,13 +1052,13 @@
       <c r="A48" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="8">
         <v>-3.904671</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D48" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1032,10 +1066,10 @@
       <c r="A49" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="8">
         <v>-3.904671</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1045,7 +1079,7 @@
       <c r="D50" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1053,25 +1087,25 @@
       <c r="A51" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="13">
         <v>400.78719999999998</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="14"/>
+      <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52" s="14">
         <v>5</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1084,26 +1118,26 @@
       <c r="A54" t="s">
         <v>33</v>
       </c>
-      <c r="B54" s="6">
+      <c r="B54" s="13">
         <f>1/(digigain)*1000000</f>
         <v>1048218.0293501049</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="14"/>
+      <c r="D54" s="6"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>34</v>
       </c>
-      <c r="B55" s="11">
+      <c r="B55" s="14">
         <v>1</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1116,13 +1150,13 @@
       <c r="A57" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="13">
         <v>1</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="D57" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1130,13 +1164,13 @@
       <c r="A58" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="11">
+      <c r="B58" s="14">
         <v>1</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D58" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1150,20 +1184,20 @@
       <c r="A60" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B60" s="16">
         <f>B54*B51*B57</f>
         <v>420112368.97274631</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C60" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D60" s="14"/>
+      <c r="D60" s="6"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
       <c r="E62" s="4" t="s">
         <v>48</v>
       </c>
@@ -1172,7 +1206,7 @@
       <c r="A63" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="8" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1180,10 +1214,10 @@
       <c r="A64" t="s">
         <v>16</v>
       </c>
-      <c r="B64" s="10">
+      <c r="B64" s="15">
         <v>90</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1191,10 +1225,10 @@
       <c r="A65" t="s">
         <v>28</v>
       </c>
-      <c r="B65" s="10">
+      <c r="B65" s="15">
         <v>0</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1202,15 +1236,20 @@
       <c r="A66" t="s">
         <v>18</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="8">
         <v>130.19999999999999</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="1"/>
+      <c r="A67" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="C67" s="1"/>
       <c r="D67" s="4" t="s">
         <v>19</v>
@@ -1220,7 +1259,7 @@
       <c r="A68" t="s">
         <v>21</v>
       </c>
-      <c r="B68" s="7">
+      <c r="B68" s="11">
         <v>2</v>
       </c>
       <c r="C68" s="1"/>
@@ -1229,11 +1268,11 @@
       <c r="A69" t="s">
         <v>50</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" s="11">
         <v>1</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="14" t="s">
+      <c r="D69" s="6" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1241,13 +1280,13 @@
       <c r="A70" t="s">
         <v>23</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="8">
         <v>-4.9842000000000004</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C70" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D70" s="14" t="s">
+      <c r="D70" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1255,10 +1294,10 @@
       <c r="A71" t="s">
         <v>24</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="8">
         <v>-4.9842000000000004</v>
       </c>
-      <c r="C71" s="9" t="s">
+      <c r="C71" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1268,7 +1307,7 @@
       <c r="D72" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E72" s="14" t="s">
+      <c r="E72" s="6" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1276,25 +1315,25 @@
       <c r="A73" t="s">
         <v>0</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" s="13">
         <v>379.62880000000001</v>
       </c>
-      <c r="C73" s="14" t="s">
+      <c r="C73" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D73" s="14"/>
+      <c r="D73" s="6"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>3</v>
       </c>
-      <c r="B74" s="11">
+      <c r="B74" s="14">
         <v>5</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C74" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D74" s="14" t="s">
+      <c r="D74" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1307,26 +1346,26 @@
       <c r="A76" t="s">
         <v>33</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="13">
         <f>1/(digigain)*1000000</f>
         <v>1048218.0293501049</v>
       </c>
-      <c r="C76" s="14" t="s">
+      <c r="C76" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D76" s="14"/>
+      <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>34</v>
       </c>
-      <c r="B77" s="11">
+      <c r="B77" s="14">
         <v>1</v>
       </c>
-      <c r="C77" s="14" t="s">
+      <c r="C77" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D77" s="14" t="s">
+      <c r="D77" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1339,13 +1378,13 @@
       <c r="A79" t="s">
         <v>33</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="13">
         <v>1</v>
       </c>
-      <c r="C79" s="14" t="s">
+      <c r="C79" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D79" s="14" t="s">
+      <c r="D79" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1353,13 +1392,13 @@
       <c r="A80" t="s">
         <v>34</v>
       </c>
-      <c r="B80" s="11">
+      <c r="B80" s="14">
         <v>1</v>
       </c>
-      <c r="C80" s="14" t="s">
+      <c r="C80" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D80" s="14" t="s">
+      <c r="D80" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1373,11 +1412,11 @@
       <c r="A82" t="s">
         <v>5</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="16">
         <f>B76*B73*B79</f>
         <v>397933752.62054509</v>
       </c>
-      <c r="C82" s="14" t="s">
+      <c r="C82" s="6" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>